<commit_message>
updating Python DA, preprocessing Airbnb and timeseries
</commit_message>
<xml_diff>
--- a/Airbnb_Analysis.xlsx
+++ b/Airbnb_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhara\MachineLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A25E3F3-4392-47E9-87EE-8C007DCAA1EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C900EC3-7320-4207-BA92-50913A71AC81}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E526F4B5-D2F2-44EB-AE2D-A9D623E9476F}"/>
   </bookViews>
@@ -394,7 +394,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +404,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -459,6 +477,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,7 +807,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A41:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +838,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -825,8 +854,12 @@
       <c r="E2" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F2" t="str">
+        <f>"'"&amp;A2&amp;"',"</f>
+        <v>'ID',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -842,8 +875,12 @@
       <c r="E3" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F66" si="0">"'"&amp;A3&amp;"',"</f>
+        <v>'Listing_Url',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
@@ -859,8 +896,12 @@
       <c r="E4" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Scrape_ID',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -876,8 +917,12 @@
       <c r="E5" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>'Last_Scraped',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -892,6 +937,10 @@
       </c>
       <c r="E6" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>'Name',</v>
       </c>
     </row>
     <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -910,6 +959,10 @@
       <c r="E7" t="s">
         <v>38</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Summary',</v>
+      </c>
     </row>
     <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -927,8 +980,12 @@
       <c r="E8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>'Space',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -944,8 +1001,12 @@
       <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>'Description',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -960,6 +1021,10 @@
       </c>
       <c r="E10" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>'Experiences_Offered',</v>
       </c>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -978,8 +1043,12 @@
       <c r="E11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>'Neighborhood_Overview',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -995,8 +1064,12 @@
       <c r="E12" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>'Notes',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1012,8 +1085,12 @@
       <c r="E13" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Transit',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1028,6 +1105,10 @@
       </c>
       <c r="E14" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>'Access',</v>
       </c>
     </row>
     <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
@@ -1046,8 +1127,12 @@
       <c r="E15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>'Interaction',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -1063,8 +1148,12 @@
       <c r="E16" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>'House_Rules',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
@@ -1080,8 +1169,12 @@
       <c r="E17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>'Thumbnail_Url',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1097,8 +1190,12 @@
       <c r="E18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>'Medium_Url',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1114,8 +1211,12 @@
       <c r="E19" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>'Picture_Url',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -1131,8 +1232,12 @@
       <c r="E20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>'XL_Picture_Url',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
@@ -1145,11 +1250,15 @@
       <c r="D21" s="2">
         <v>12995</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_ID',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1165,8 +1274,12 @@
       <c r="E22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_URL',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
@@ -1182,9 +1295,13 @@
       <c r="E23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Name',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1199,9 +1316,13 @@
       <c r="E24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Since',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1216,8 +1337,12 @@
       <c r="E25" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Location',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -1233,9 +1358,13 @@
       <c r="E26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_About',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1250,9 +1379,13 @@
       <c r="E27" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Response_Time',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1267,8 +1400,12 @@
       <c r="E28" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Response_Rate',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
@@ -1284,8 +1421,12 @@
       <c r="E29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Thumbnail_Url',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>70</v>
       </c>
@@ -1301,9 +1442,13 @@
       <c r="E30" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Picture_Url',</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1318,9 +1463,13 @@
       <c r="E31" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Neighbourhood',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1335,9 +1484,13 @@
       <c r="E32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Listings_Count',</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1352,9 +1505,13 @@
       <c r="E33" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Total_Listings_Count',</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1369,8 +1526,12 @@
       <c r="E34" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>'Host_Verifications',</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -1383,12 +1544,16 @@
       <c r="D35" s="2">
         <v>7113</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>'Street',</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1403,9 +1568,13 @@
       <c r="E36" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>'Neighbourhood',</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1420,9 +1589,13 @@
       <c r="E37" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>'Neighbourhood_Cleansed',</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1437,9 +1610,13 @@
       <c r="E38" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>'City',</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1454,8 +1631,12 @@
       <c r="E39" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>'State',</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -1471,9 +1652,13 @@
       <c r="E40" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>'Zipcode',</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1488,9 +1673,13 @@
       <c r="E41" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>'Market',</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1505,8 +1694,12 @@
       <c r="E42" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>'Smart_Location',</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>76</v>
       </c>
@@ -1522,8 +1715,12 @@
       <c r="E43" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>'Country_Code',</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>21</v>
       </c>
@@ -1539,9 +1736,13 @@
       <c r="E44" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>'Country',</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1556,9 +1757,13 @@
       <c r="E45" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>'Latitude',</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1573,9 +1778,13 @@
       <c r="E46" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>'Longitude',</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
         <v>77</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1590,9 +1799,13 @@
       <c r="E47" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>'Property_Type',</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -1607,9 +1820,13 @@
       <c r="E48" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>'Room_Type',</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -1624,9 +1841,13 @@
       <c r="E49" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>'Accommodates',</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -1641,9 +1862,13 @@
       <c r="E50" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>'Bathrooms',</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -1658,9 +1883,13 @@
       <c r="E51" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>'Bedrooms',</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -1675,9 +1904,13 @@
       <c r="E52" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>'Beds',</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -1692,9 +1925,13 @@
       <c r="E53" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>'Bed_Type',</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -1709,8 +1946,12 @@
       <c r="E54" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>'Amenities',</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>80</v>
       </c>
@@ -1726,9 +1967,13 @@
       <c r="E55" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>'Square_Feet',</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -1743,9 +1988,13 @@
       <c r="E56" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>'Price',</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
         <v>81</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -1760,9 +2009,13 @@
       <c r="E57" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>'Weekly_Price',</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
         <v>82</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -1777,9 +2030,13 @@
       <c r="E58" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>'Monthly_Price',</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
         <v>83</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -1794,9 +2051,13 @@
       <c r="E59" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>'Security_Deposit',</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -1811,9 +2072,13 @@
       <c r="E60" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>'Cleaning_Fee',</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
         <v>85</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -1828,9 +2093,13 @@
       <c r="E61" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>'Guests_Included',</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
         <v>86</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -1842,12 +2111,16 @@
       <c r="D62" s="2">
         <v>86</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>'Extra_People',</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -1859,12 +2132,16 @@
       <c r="D63" s="2">
         <v>38</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>'Minimum_Nights',</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -1876,11 +2153,15 @@
       <c r="D64" s="2">
         <v>130</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>'Maximum_Nights',</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>89</v>
       </c>
@@ -1896,9 +2177,13 @@
       <c r="E65" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>'Calendar_Updated',</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="10" t="s">
         <v>90</v>
       </c>
       <c r="B66" s="2" t="s">
@@ -1913,9 +2198,13 @@
       <c r="E66" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>'Availability_30',</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -1930,9 +2219,13 @@
       <c r="E67" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="F67" t="str">
+        <f t="shared" ref="F67:F86" si="1">"'"&amp;A67&amp;"',"</f>
+        <v>'Availability_60',</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="10" t="s">
         <v>92</v>
       </c>
       <c r="B68" s="2" t="s">
@@ -1947,9 +2240,13 @@
       <c r="E68" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+      <c r="F68" t="str">
+        <f t="shared" si="1"/>
+        <v>'Availability_90',</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B69" s="2" t="s">
@@ -1964,8 +2261,12 @@
       <c r="E69" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F69" t="str">
+        <f t="shared" si="1"/>
+        <v>'Availability_365',</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>94</v>
       </c>
@@ -1981,9 +2282,13 @@
       <c r="E70" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+      <c r="F70" t="str">
+        <f t="shared" si="1"/>
+        <v>'Calendar_last_Scraped',</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -1998,9 +2303,13 @@
       <c r="E71" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+      <c r="F71" t="str">
+        <f t="shared" si="1"/>
+        <v>'Number_of_Reviews',</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="10" t="s">
         <v>96</v>
       </c>
       <c r="B72" s="2" t="s">
@@ -2015,9 +2324,13 @@
       <c r="E72" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+      <c r="F72" t="str">
+        <f t="shared" si="1"/>
+        <v>'First_Review',</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="10" t="s">
         <v>97</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -2032,9 +2345,13 @@
       <c r="E73" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="F73" t="str">
+        <f t="shared" si="1"/>
+        <v>'Last_Review',</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="10" t="s">
         <v>98</v>
       </c>
       <c r="B74" s="2" t="s">
@@ -2049,9 +2366,13 @@
       <c r="E74" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+      <c r="F74" t="str">
+        <f t="shared" si="1"/>
+        <v>'Review_Scores_Rating',</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
         <v>99</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -2066,9 +2387,13 @@
       <c r="E75" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="F75" t="str">
+        <f t="shared" si="1"/>
+        <v>'Review_Scores_Accuracy',</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="10" t="s">
         <v>100</v>
       </c>
       <c r="B76" s="2" t="s">
@@ -2080,12 +2405,16 @@
       <c r="D76" s="2">
         <v>9</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+      <c r="F76" t="str">
+        <f t="shared" si="1"/>
+        <v>'Review_Scores_Cleanliness',</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="10" t="s">
         <v>101</v>
       </c>
       <c r="B77" s="2" t="s">
@@ -2097,12 +2426,16 @@
       <c r="D77" s="2">
         <v>8</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+      <c r="F77" t="str">
+        <f t="shared" si="1"/>
+        <v>'Review_Scores_Checkin',</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="10" t="s">
         <v>102</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -2114,12 +2447,16 @@
       <c r="D78" s="2">
         <v>8</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+      <c r="F78" t="str">
+        <f t="shared" si="1"/>
+        <v>'Review_Scores_Communication',</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="10" t="s">
         <v>103</v>
       </c>
       <c r="B79" s="2" t="s">
@@ -2131,12 +2468,16 @@
       <c r="D79" s="2">
         <v>8</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+      <c r="F79" t="str">
+        <f t="shared" si="1"/>
+        <v>'Review_Scores_Location',</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="10" t="s">
         <v>104</v>
       </c>
       <c r="B80" s="2" t="s">
@@ -2148,11 +2489,15 @@
       <c r="D80" s="2">
         <v>9</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F80" t="str">
+        <f t="shared" si="1"/>
+        <v>'Review_Scores_Value',</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>105</v>
       </c>
@@ -2168,9 +2513,13 @@
       <c r="E81" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+      <c r="F81" t="str">
+        <f t="shared" si="1"/>
+        <v>'Jurisdiction_Names',</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="10" t="s">
         <v>106</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -2185,9 +2534,13 @@
       <c r="E82" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+      <c r="F82" t="str">
+        <f t="shared" si="1"/>
+        <v>'Cancellation_Policy',</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="10" t="s">
         <v>107</v>
       </c>
       <c r="B83" s="2" t="s">
@@ -2202,9 +2555,13 @@
       <c r="E83" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+      <c r="F83" t="str">
+        <f t="shared" si="1"/>
+        <v>'Calculated_host_listings_count',</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="10" t="s">
         <v>108</v>
       </c>
       <c r="B84" s="2" t="s">
@@ -2219,9 +2576,13 @@
       <c r="E84" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="F84" t="str">
+        <f t="shared" si="1"/>
+        <v>'Reviews_per_Month',</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B85" s="2" t="s">
@@ -2236,9 +2597,13 @@
       <c r="E85" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+      <c r="F85" t="str">
+        <f t="shared" si="1"/>
+        <v>'Geolocation',</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B86" s="2" t="s">
@@ -2252,17 +2617,21 @@
       </c>
       <c r="E86" t="s">
         <v>44</v>
+      </c>
+      <c r="F86" t="str">
+        <f t="shared" si="1"/>
+        <v>'Features',</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F86" xr:uid="{9A68F719-D1A1-4DE1-A628-D6B505239857}">
     <filterColumn colId="4">
       <filters>
-        <filter val="consider binning and descritization"/>
-        <filter val="consider binning and descritization,na to 0"/>
+        <filter val="None"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>